<commit_message>
Update the project workload plan
</commit_message>
<xml_diff>
--- a/final-project-workload-plan.xlsx
+++ b/final-project-workload-plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t xml:space="preserve">FILL IN THE BLUE BOXES ONLY</t>
   </si>
@@ -43,10 +43,13 @@
     <t xml:space="preserve">member 3</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;student id&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;student name&gt;</t>
+    <t xml:space="preserve">Kuba Trzykowski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marko Putnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anton Kalpakchiev</t>
   </si>
   <si>
     <t xml:space="preserve">basic features</t>
@@ -137,7 +140,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,49 +164,25 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -222,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -252,13 +231,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top style="hair"/>
@@ -305,136 +277,112 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,39 +459,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="48.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="54.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="8.73"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -552,21 +503,21 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -574,48 +525,48 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="6" t="n">
+        <v>5532949</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>5497760</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>5531063</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
       <c r="G7" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>0.5</v>
@@ -627,16 +578,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G8" s="8" t="n">
         <f aca="false">SUM(D8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>2</v>
@@ -645,25 +596,25 @@
         <v>0</v>
       </c>
       <c r="E9" s="13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F9" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="8" t="n">
         <f aca="false">SUM(D9:F9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E10" s="13" t="n">
         <v>0</v>
@@ -673,12 +624,12 @@
       </c>
       <c r="G10" s="8" t="n">
         <f aca="false">SUM(D10:F10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="16" t="n">
         <v>4</v>
@@ -690,22 +641,22 @@
         <v>0</v>
       </c>
       <c r="F11" s="14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G11" s="8" t="n">
         <f aca="false">SUM(D11:F11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="16" t="n">
         <v>5</v>
       </c>
       <c r="D12" s="13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E12" s="13" t="n">
         <v>0</v>
@@ -715,35 +666,35 @@
       </c>
       <c r="G12" s="8" t="n">
         <f aca="false">SUM(D12:F12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D13" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F13" s="14" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="8" t="n">
         <f aca="false">SUM(D13:F13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="13" t="n">
@@ -753,323 +704,323 @@
         <v>0</v>
       </c>
       <c r="F14" s="14" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G14" s="8" t="n">
         <f aca="false">SUM(D14:F14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="16" t="n">
         <v>1.5</v>
       </c>
       <c r="D15" s="13" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="13" t="n">
-        <v>0</v>
+        <v>66.66666666666</v>
       </c>
       <c r="F15" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G15" s="8" t="n">
         <f aca="false">SUM(D15:F15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="21" t="n">
+        <v>99.99999999996</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5"/>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="17" t="n">
         <f aca="false">SUM(C8:C15)</f>
         <v>18</v>
       </c>
-      <c r="D16" s="22" t="n">
+      <c r="D16" s="18" t="n">
         <f aca="false">SUMPRODUCT(C8:C15,D8:D15)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" s="18" t="n">
         <f aca="false">SUMPRODUCT($C8:$C15,E8:E15)/100</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="22" t="n">
+        <v>5.9999999999999</v>
+      </c>
+      <c r="F16" s="18" t="n">
         <f aca="false">SUMPRODUCT($C8:$C15,F8:F15)/100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>8</v>
+        <v>5.9999999999995</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5"/>
+      <c r="B18" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
       <c r="G18" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5"/>
       <c r="B19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="24" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D19" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <v>0</v>
+      <c r="D19" s="14" t="n">
+        <v>33.3333333334</v>
+      </c>
+      <c r="E19" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F19" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G19" s="8" t="n">
         <f aca="false">SUM(D19:F19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="24" t="n">
+        <v>21</v>
+      </c>
+      <c r="C20" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D20" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13" t="n">
-        <v>0</v>
+      <c r="D20" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E20" s="14" t="n">
+        <v>33.3333333334</v>
       </c>
       <c r="F20" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G20" s="8" t="n">
         <f aca="false">SUM(D20:F20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C21" s="12" t="n">
         <v>2.5</v>
       </c>
-      <c r="D21" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="13" t="n">
-        <v>0</v>
+      <c r="D21" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E21" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F21" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333334</v>
       </c>
       <c r="G21" s="8" t="n">
         <f aca="false">SUM(D21:F21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C22" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D22" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13" t="n">
-        <v>0</v>
+      <c r="D22" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E22" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F22" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G22" s="8" t="n">
         <f aca="false">SUM(D22:F22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="24" t="n">
+        <v>24</v>
+      </c>
+      <c r="C23" s="12" t="n">
         <v>0.5</v>
       </c>
-      <c r="D23" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13" t="n">
-        <v>0</v>
+      <c r="D23" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E23" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F23" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G23" s="8" t="n">
         <f aca="false">SUM(D23:F23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="24" t="n">
+        <v>25</v>
+      </c>
+      <c r="C24" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="D24" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="13" t="n">
-        <v>0</v>
+      <c r="D24" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E24" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F24" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G24" s="8" t="n">
         <f aca="false">SUM(D24:F24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="24" t="n">
+        <v>26</v>
+      </c>
+      <c r="C25" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D25" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="13" t="n">
-        <v>0</v>
+      <c r="D25" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E25" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F25" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G25" s="8" t="n">
         <f aca="false">SUM(D25:F25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="24" t="n">
+        <v>27</v>
+      </c>
+      <c r="C26" s="12" t="n">
         <v>2.5</v>
       </c>
-      <c r="D26" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="13" t="n">
-        <v>0</v>
+      <c r="D26" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E26" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F26" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G26" s="8" t="n">
         <f aca="false">SUM(D26:F26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="24" t="n">
+        <v>28</v>
+      </c>
+      <c r="C27" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="D27" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13" t="n">
-        <v>0</v>
+      <c r="D27" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E27" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F27" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G27" s="8" t="n">
         <f aca="false">SUM(D27:F27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="24" t="n">
+        <v>29</v>
+      </c>
+      <c r="C28" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="D28" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="13" t="n">
-        <v>0</v>
+      <c r="D28" s="14" t="n">
+        <v>33.3333333333</v>
+      </c>
+      <c r="E28" s="14" t="n">
+        <v>33.3333333333</v>
       </c>
       <c r="F28" s="14" t="n">
-        <v>0</v>
+        <v>33.3333333333</v>
       </c>
       <c r="G28" s="8" t="n">
         <f aca="false">SUM(D28:F28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="27" t="n">
+        <v>99.9999999999</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="21" t="n">
         <f aca="false">SUM(C19:C28)</f>
         <v>18</v>
       </c>
-      <c r="D29" s="22" t="n">
+      <c r="D29" s="18" t="n">
         <f aca="false">SUMPRODUCT($C19:$C28,D19:D28)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="22" t="n">
+        <v>5.9999999999955</v>
+      </c>
+      <c r="E29" s="18" t="n">
         <f aca="false">SUMPRODUCT($C19:$C28,E19:E28)/100</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="22" t="n">
+        <v>5.9999999999955</v>
+      </c>
+      <c r="F29" s="18" t="n">
         <f aca="false">SUMPRODUCT($C19:$C28,F19:F28)/100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30" t="n">
+        <v>5.9999999999965</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24" t="n">
         <f aca="false">D$16+D29</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="30" t="n">
+        <v>11.9999999999955</v>
+      </c>
+      <c r="E31" s="24" t="n">
         <f aca="false">E$16+E29</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="31" t="n">
+        <v>11.9999999999954</v>
+      </c>
+      <c r="F31" s="25" t="n">
         <f aca="false">F$16+F29</f>
-        <v>0</v>
+        <v>11.999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1088,31 +1039,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
-        <v>30</v>
+      <c r="A1" s="26" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
-        <v>31</v>
+      <c r="A2" s="26" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
-        <v>32</v>
+      <c r="A3" s="26" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>